<commit_message>
add image list kewords
</commit_message>
<xml_diff>
--- a/doc/test.xlsx
+++ b/doc/test.xlsx
@@ -413,9 +413,9 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -507,7 +507,6 @@
           <t>Warthin’s tumor.</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -548,7 +547,6 @@
       <c r="H3" t="n">
         <v>1</v>
       </c>
-      <c r="I3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -589,7 +587,6 @@
       <c r="H4" t="n">
         <v>4</v>
       </c>
-      <c r="I4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -630,7 +627,6 @@
       <c r="H5" t="n">
         <v>1</v>
       </c>
-      <c r="I5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -663,7 +659,6 @@
           <t>أول أكسيد الكربون.</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr"/>
       <c r="H6" t="n">
         <v>1</v>
       </c>
@@ -689,7 +684,6 @@
           <t>الطحال.</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr"/>
       <c r="H7" t="n">
         <v>1</v>
       </c>
@@ -733,7 +727,6 @@
       <c r="H8" t="n">
         <v>4</v>
       </c>
-      <c r="I8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -766,7 +759,6 @@
           <t>It allows for enrollment once patients require nursing home level of care.</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr"/>
       <c r="H9" t="n">
         <v>4</v>
       </c>
@@ -804,45 +796,8 @@
           <t>Transfer to hospice.</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr"/>
       <c r="H10" t="n">
         <v>3</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>mc</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>An 81-year-old man presents to the hospital after his wife finds him febrile and confused at home. She states he has been coughing ever since their children and school-aged grandchildren visited a week ago to celebrate their 60th wedding anniversary. An X-ray in the emergency room demonstrated pneumonia in the right middle lobe, and he is admitted to the hospital and started on antibiotics. While hospitalized, the patient’s mental status worsens, and he is unable to recognize where he is and cannot recall his wife’s name.  
-Which of the following bedside tests has demonstrated the highest sensitivity and specificity in evaluating this patient’s condition?</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Mini-Mental Status Exam.</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Confusion Assessment Method.</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>Digit Span Test.</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>The Vigilance “A” test.</t>
-        </is>
-      </c>
-      <c r="H11" t="n">
-        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>